<commit_message>
updated sprint backlog + sprint burndown chart
</commit_message>
<xml_diff>
--- a/Team/Team03/Sprint Backlog/Sprint Backlog.xlsx
+++ b/Team/Team03/Sprint Backlog/Sprint Backlog.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy Lee\Documents\Tugas Kuliah\Agile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!!Documents\Learning\Semester 4\Agile Software Development\Personal Report\Team\Team03\Sprint Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="12 Mei (1)" sheetId="1" r:id="rId1"/>
-    <sheet name="12 Mei (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="31 Maret (1)" sheetId="3" r:id="rId3"/>
-    <sheet name="31 Maret (2)" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint Backlog" sheetId="6" r:id="rId1"/>
+    <sheet name="Sprint Burndown Chart" sheetId="5" r:id="rId2"/>
+    <sheet name="12 Mei (1)" sheetId="1" r:id="rId3"/>
+    <sheet name="12 Mei (2)" sheetId="2" r:id="rId4"/>
+    <sheet name="31 Maret (1)" sheetId="3" r:id="rId5"/>
+    <sheet name="31 Maret (2)" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,6 +34,270 @@
     <author>Tommy Lee</author>
   </authors>
   <commentList>
+    <comment ref="F10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Design</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Database</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Backend
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tester</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Design</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Backend</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tester
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Design</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Database</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Backend</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Testing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Design</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Database</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Backend</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Testing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Design</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Backend</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tester</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tommy Lee</author>
+  </authors>
+  <commentList>
     <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
@@ -291,7 +557,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="45">
   <si>
     <t>Task</t>
   </si>
@@ -414,6 +680,18 @@
   </si>
   <si>
     <t>DJ, KV, YA, OI</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
   </si>
 </sst>
 </file>
@@ -444,7 +722,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -493,15 +771,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -528,8 +837,986 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="id-ID"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog'!$B$15:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7F74-4812-9B98-5EB1ED9B14EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="224670312"/>
+        <c:axId val="224670640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="224670312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DAYS WITHIN A SPRINT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="224670640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="224670640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ESTIMATED</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> EFFORT-HOURS REMAINING</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="224670312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Bagan 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -791,10 +2078,429 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1">
+        <v>4</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>6</v>
+      </c>
+      <c r="J14" s="1">
+        <v>4</v>
+      </c>
+      <c r="K14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" ref="B15:G15" si="0">SUM(B2:B14)</f>
+        <v>57</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" ref="H15:K15" si="1">SUM(H2:H14)</f>
+        <v>15</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G6" sqref="A2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,14 +2549,20 @@
       <c r="E2" s="1">
         <v>2</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
       <c r="C3" s="1">
         <v>4</v>
       </c>
@@ -860,15 +2572,23 @@
       <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
       <c r="D4" s="1">
         <v>4</v>
       </c>
@@ -886,8 +2606,12 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
       <c r="D5" s="1">
         <v>4</v>
       </c>
@@ -905,9 +2629,15 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
       <c r="E6" s="1">
         <v>6</v>
       </c>
@@ -953,12 +2683,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,10 +2710,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1052,10 +2782,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -1124,10 +2854,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
@@ -1196,10 +2926,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
@@ -1268,10 +2998,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
@@ -1378,12 +3108,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,11 +3312,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1696,10 +3426,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="1">
         <f>SUM(C2:C9)</f>
         <v>57</v>

</xml_diff>